<commit_message>
use logger and fix data types. bump version
</commit_message>
<xml_diff>
--- a/spec/files/setup_version_2.xlsx
+++ b/spec/files/setup_version_2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="492">
   <si>
     <t>type</t>
   </si>
@@ -1499,6 +1499,9 @@
   </si>
   <si>
     <t>Analysis Type</t>
+  </si>
+  <si>
+    <t>Tolerance</t>
   </si>
 </sst>
 </file>
@@ -2952,9 +2955,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2963,6 +2963,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1285">
@@ -4583,10 +4586,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4601,7 +4604,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="22"/>
-      <c r="B1" s="26"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
       <c r="E1" s="23" t="s">
@@ -4612,7 +4615,7 @@
       <c r="A2" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
@@ -4632,7 +4635,7 @@
       <c r="A4" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>458</v>
       </c>
       <c r="C4" s="3" t="str">
@@ -4651,7 +4654,7 @@
       <c r="A5" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>458</v>
       </c>
       <c r="C5" s="3" t="str">
@@ -4670,7 +4673,7 @@
       <c r="A7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="12"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -4679,7 +4682,7 @@
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -4690,7 +4693,7 @@
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>482</v>
       </c>
     </row>
@@ -4698,7 +4701,7 @@
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>483</v>
       </c>
     </row>
@@ -4706,7 +4709,7 @@
       <c r="A12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="27"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="14" t="s">
@@ -4717,7 +4720,7 @@
       <c r="A13" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4725,7 +4728,7 @@
       <c r="A15" s="12" t="s">
         <v>486</v>
       </c>
-      <c r="B15" s="27"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="14" t="s">
@@ -4736,7 +4739,7 @@
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="27" t="s">
         <v>489</v>
       </c>
     </row>
@@ -4744,7 +4747,7 @@
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="27">
         <v>100</v>
       </c>
     </row>
@@ -4752,78 +4755,87 @@
       <c r="A18" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="27">
         <v>20</v>
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A20" s="12" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B19" s="27">
+        <v>0.115</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A21" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B21" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="14"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
+      <c r="D21" s="12"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B22" s="27" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A23" s="12" t="s">
+    <row r="24" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A24" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B24" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C24" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D24" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E24" s="14" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:5" ht="28">
+      <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B25" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D25" s="24" t="s">
         <v>484</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A26" s="12" t="s">
+    <row r="27" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A27" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B27" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C27" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="14"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4898,14 +4910,14 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="25" t="s">
+      <c r="Q1" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
     </row>
     <row r="2" spans="1:22" s="9" customFormat="1" ht="15">
       <c r="A2" s="9" t="s">

</xml_diff>